<commit_message>
:+1: Upgrade to use RadCombobox
</commit_message>
<xml_diff>
--- a/Source/Website/DesktopModules/Modules/EmployeeManagement/Assets/Template/Template_Employee.xlsx
+++ b/Source/Website/DesktopModules/Modules/EmployeeManagement/Assets/Template/Template_Employee.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huynhhuuloc\Desktop\TanTran\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VietBank\Portal\Source\Website\DesktopModules\Modules\EmployeeManagement\Assets\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,34 +101,34 @@
     <t>Trần Nhật Phương</t>
   </si>
   <si>
-    <t>15/3/1994</t>
-  </si>
-  <si>
     <t>Chánh văn phòng Ban TGD</t>
   </si>
   <si>
     <t>VĂN PHÒNG BAN TỔNG GIÁM ĐỐC</t>
   </si>
   <si>
-    <t>1/6/2017</t>
-  </si>
-  <si>
-    <t>20/12/2015</t>
-  </si>
-  <si>
     <t>Cục ĐKQL cư trú và DLQG về dân cư</t>
   </si>
   <si>
     <t>0123465789</t>
   </si>
   <si>
-    <t>tnphuong@vietbank.com.vn</t>
+    <t>19940315</t>
+  </si>
+  <si>
+    <t>20170601</t>
+  </si>
+  <si>
+    <t>20151220</t>
+  </si>
+  <si>
+    <t>trannhatphuong@vietbank.com.vn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,19 +201,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -499,28 +495,29 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -530,7 +527,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -548,10 +545,10 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -560,7 +557,7 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -586,17 +583,17 @@
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>20</v>
@@ -604,11 +601,11 @@
       <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>27</v>
+      <c r="I2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>19</v>
@@ -616,22 +613,22 @@
       <c r="L2" s="2">
         <v>123456789</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>28</v>
+      <c r="M2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O2" s="2">
         <v>123456789</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="3">
+      <c r="P2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="4">
         <v>1122</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>